<commit_message>
clean du code de details de requete
</commit_message>
<xml_diff>
--- a/FichesTemps/LouisGarceauSemaine4.xlsx
+++ b/FichesTemps/LouisGarceauSemaine4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8345809-5BAF-412E-8DB5-C972237191F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F720E89-FCF7-4953-A509-FF865E3BE517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="88">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -401,6 +401,15 @@
   </si>
   <si>
     <t>Tentative de fonctionnement de print avec react native</t>
+  </si>
+  <si>
+    <t>Rencontre avec la cliente pour s'assurer du bon fonctionnement de l'application</t>
+  </si>
+  <si>
+    <t>Finition de l'affichage de résultats d'une requête</t>
+  </si>
+  <si>
+    <t>Changements faits sur l'affichage de résultat pour qu'il soit similaire à celui de l'ajout de résultat</t>
   </si>
 </sst>
 </file>
@@ -1779,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1873,7 +1882,7 @@
       </c>
       <c r="C9" s="41">
         <f>SUM(C11:C463)</f>
-        <v>10.5</v>
+        <v>14</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>64</v>
@@ -2005,22 +2014,40 @@
       <c r="D20" s="43"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
+      <c r="A21" s="42">
+        <v>44973</v>
+      </c>
       <c r="B21" s="46"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="46"/>
+      <c r="C21" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
+      <c r="A22" s="42">
+        <v>44973</v>
+      </c>
       <c r="B22" s="46"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="46"/>
+      <c r="C22" s="47">
+        <v>1</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
+      <c r="A23" s="42">
+        <v>44973</v>
+      </c>
       <c r="B23" s="46"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="46"/>
+      <c r="C23" s="47">
+        <v>1</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="42"/>

</xml_diff>

<commit_message>
fix du test unitaire de création de requête
</commit_message>
<xml_diff>
--- a/FichesTemps/LouisGarceauSemaine4.xlsx
+++ b/FichesTemps/LouisGarceauSemaine4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F720E89-FCF7-4953-A509-FF865E3BE517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23786CB0-B9D9-4ED4-A852-3C344F98D7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="89">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t>Changements faits sur l'affichage de résultat pour qu'il soit similaire à celui de l'ajout de résultat</t>
+  </si>
+  <si>
+    <t>Encore fix du test unitaire de création de requête qui ne recevait pas le result</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1792,7 @@
   <dimension ref="A1:F463"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1882,7 +1885,7 @@
       </c>
       <c r="C9" s="41">
         <f>SUM(C11:C463)</f>
-        <v>14</v>
+        <v>14.25</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>64</v>
@@ -2050,10 +2053,16 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="42"/>
+      <c r="A24" s="42">
+        <v>44973</v>
+      </c>
       <c r="B24" s="46"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="46"/>
+      <c r="C24" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="45"/>

</xml_diff>

<commit_message>
fix de création de requête
</commit_message>
<xml_diff>
--- a/FichesTemps/LouisGarceauSemaine4.xlsx
+++ b/FichesTemps/LouisGarceauSemaine4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23786CB0-B9D9-4ED4-A852-3C344F98D7EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C813BEE5-326B-4155-9EB4-66167EBAAE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="91">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -406,13 +406,19 @@
     <t>Rencontre avec la cliente pour s'assurer du bon fonctionnement de l'application</t>
   </si>
   <si>
-    <t>Finition de l'affichage de résultats d'une requête</t>
-  </si>
-  <si>
     <t>Changements faits sur l'affichage de résultat pour qu'il soit similaire à celui de l'ajout de résultat</t>
   </si>
   <si>
     <t>Encore fix du test unitaire de création de requête qui ne recevait pas le result</t>
+  </si>
+  <si>
+    <t>Finition de l'affichage de résultats d'une requête (style et affichage demandé)</t>
+  </si>
+  <si>
+    <t>Recherche sur le changement de nom d'application sur windows d'une application React native</t>
+  </si>
+  <si>
+    <t>Fix de l'affichage de requêtes en ordre de date</t>
   </si>
 </sst>
 </file>
@@ -1791,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1885,7 +1891,7 @@
       </c>
       <c r="C9" s="41">
         <f>SUM(C11:C463)</f>
-        <v>14.25</v>
+        <v>16</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>64</v>
@@ -2025,7 +2031,7 @@
         <v>1.5</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2046,10 +2052,10 @@
       </c>
       <c r="B23" s="46"/>
       <c r="C23" s="47">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D23" s="46" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2058,23 +2064,35 @@
       </c>
       <c r="B24" s="46"/>
       <c r="C24" s="47">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D24" s="46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="45"/>
+      <c r="A25" s="42">
+        <v>44973</v>
+      </c>
       <c r="B25" s="46"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="46"/>
+      <c r="C25" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="42"/>
+      <c r="A26" s="42">
+        <v>44973</v>
+      </c>
       <c r="B26" s="46"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="46"/>
+      <c r="C26" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="42"/>

</xml_diff>

<commit_message>
ajout du message quand aucune analyse demandée et changements visuels
</commit_message>
<xml_diff>
--- a/FichesTemps/LouisGarceauSemaine4.xlsx
+++ b/FichesTemps/LouisGarceauSemaine4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C813BEE5-326B-4155-9EB4-66167EBAAE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B65291-5A98-42FA-B187-9C14CE438580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="92">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -419,6 +419,9 @@
   </si>
   <si>
     <t>Fix de l'affichage de requêtes en ordre de date</t>
+  </si>
+  <si>
+    <t>Ajout du message quand aucune analyse n'a été demandée pour une requête et ajustements visuels des détails de requête</t>
   </si>
 </sst>
 </file>
@@ -1797,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1891,7 +1894,7 @@
       </c>
       <c r="C9" s="41">
         <f>SUM(C11:C463)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>64</v>
@@ -2028,7 +2031,7 @@
       </c>
       <c r="B21" s="46"/>
       <c r="C21" s="47">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D21" s="46" t="s">
         <v>86</v>
@@ -2076,7 +2079,7 @@
       </c>
       <c r="B25" s="46"/>
       <c r="C25" s="47">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D25" s="46" t="s">
         <v>89</v>
@@ -2101,10 +2104,16 @@
       <c r="D27" s="46"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="42"/>
+      <c r="A28" s="42">
+        <v>44974</v>
+      </c>
       <c r="B28" s="46"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="46"/>
+      <c r="C28" s="47">
+        <v>1.25</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="42"/>

</xml_diff>

<commit_message>
ajout de messages d'erreur dans la création de dossier
</commit_message>
<xml_diff>
--- a/FichesTemps/LouisGarceauSemaine4.xlsx
+++ b/FichesTemps/LouisGarceauSemaine4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86EF18D-3172-42FC-914E-BC9497287663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3DDE41-A9AA-4E69-ABCD-E152953C440A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="95">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -425,6 +425,12 @@
   </si>
   <si>
     <t>Recherche pour voir pourquoi l'app reçoi un 500 avec la création de requête qui retourne la requête (sans succès)</t>
+  </si>
+  <si>
+    <t>Ajout du message quand aucune requête n'a été faite pour un dossier</t>
+  </si>
+  <si>
+    <t>Sexe Autre enlevé, aucune sexe par défaut et messages d'erreurs quand aucun sexe n'a été sélectionné</t>
   </si>
 </sst>
 </file>
@@ -1803,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1897,7 +1903,7 @@
       </c>
       <c r="C9" s="41">
         <f>SUM(C11:C463)</f>
-        <v>19</v>
+        <v>20.079999999999998</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>64</v>
@@ -2137,16 +2143,28 @@
       <c r="D30" s="46"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
+      <c r="A31" s="42">
+        <v>44975</v>
+      </c>
       <c r="B31" s="46"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="46"/>
+      <c r="C31" s="47">
+        <v>0.33</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="42"/>
+      <c r="A32" s="42">
+        <v>44975</v>
+      </c>
       <c r="B32" s="46"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="46"/>
+      <c r="C32" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="D32" s="46" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="42"/>

</xml_diff>

<commit_message>
reload de résultats et changements visuels
</commit_message>
<xml_diff>
--- a/FichesTemps/LouisGarceauSemaine4.xlsx
+++ b/FichesTemps/LouisGarceauSemaine4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3DDE41-A9AA-4E69-ABCD-E152953C440A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646B1257-959D-40DD-B2E7-A2298BF1966D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="98">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -431,6 +431,15 @@
   </si>
   <si>
     <t>Sexe Autre enlevé, aucune sexe par défaut et messages d'erreurs quand aucun sexe n'a été sélectionné</t>
+  </si>
+  <si>
+    <t>Netoyage général de code</t>
+  </si>
+  <si>
+    <t>Ajout du reload des résultats quand ils sont sauvegardés</t>
+  </si>
+  <si>
+    <t>Ajustements visuels de l'application (correction d'erreur et changements de détails de dossier)</t>
   </si>
 </sst>
 </file>
@@ -1809,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1903,7 +1912,7 @@
       </c>
       <c r="C9" s="41">
         <f>SUM(C11:C463)</f>
-        <v>20.079999999999998</v>
+        <v>22.08</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>64</v>
@@ -2167,10 +2176,16 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="42"/>
+      <c r="A33" s="42">
+        <v>44975</v>
+      </c>
       <c r="B33" s="46"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="46"/>
+      <c r="C33" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="46" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="42"/>
@@ -2179,16 +2194,28 @@
       <c r="D34" s="46"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="42"/>
+      <c r="A35" s="42">
+        <v>44976</v>
+      </c>
       <c r="B35" s="46"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="46"/>
+      <c r="C35" s="47">
+        <v>1</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="42"/>
+      <c r="A36" s="42">
+        <v>44976</v>
+      </c>
       <c r="B36" s="46"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="46"/>
+      <c r="C36" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="45"/>

</xml_diff>